<commit_message>
Update Data Category 1
</commit_message>
<xml_diff>
--- a/Methods-Data-Processing-Visualization/Resources-Data-Category-1-GDP-and-Final-Expenditure-Components/Initial-Datasets-1/y_gdp_exp_cli _caladj.xlsx
+++ b/Methods-Data-Processing-Visualization/Resources-Data-Category-1-GDP-and-Final-Expenditure-Components/Initial-Datasets-1/y_gdp_exp_cli _caladj.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f1b2c5bbce95d43/Bureau/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f1b2c5bbce95d43/Bureau/Github/Major-Economic-Developments-in-Turkey-1998-Mid-2024/Methods-Data-Processing-Visualization/Resources-Data-Category-1-GDP-and-Final-Expenditure-Components/Initial-Datasets-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC10486C391A45DE5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8121D715-D418-4C76-A51B-B10971B5A9A8}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC10486C391A45DE5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDB55A8B-5DA8-49EC-A2D8-A2E4C9CC8BBA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Selected" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Year</t>
   </si>
@@ -82,13 +82,7 @@
     <t>Dataset</t>
   </si>
   <si>
-    <t>Temporal aggregation of quarterly calendar adjusted series</t>
-  </si>
-  <si>
-    <t>Date of Publication of Original Dataset</t>
-  </si>
-  <si>
-    <t>Derivation</t>
+    <t>Date of Publication</t>
   </si>
 </sst>
 </file>
@@ -489,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1661,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966BB437-AF40-47AC-8457-C173BDF9295F}">
   <dimension ref="A5:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,10 +1687,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -1717,10 +1708,7 @@
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="8">
+      <c r="F6" s="8">
         <v>45537</v>
       </c>
       <c r="H6" s="6"/>

</xml_diff>